<commit_message>
SVM: last 5000 samples
</commit_message>
<xml_diff>
--- a/report/Report.xlsx
+++ b/report/Report.xlsx
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t xml:space="preserve">				</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t xml:space="preserve">Название метода </t>
   </si>
@@ -26,9 +23,6 @@
   </si>
   <si>
     <t>Точность (матожидание)</t>
-  </si>
-  <si>
-    <t>Точность (дисперсия)</t>
   </si>
   <si>
     <t>Linear, C=1</t>
@@ -40,13 +34,16 @@
     <t>Метод проверки</t>
   </si>
   <si>
-    <t>CV</t>
-  </si>
-  <si>
     <t>SVM (SVC)</t>
   </si>
   <si>
     <t>Время работы (сек)</t>
+  </si>
+  <si>
+    <t>CV, 5</t>
+  </si>
+  <si>
+    <t>Доверительный интервал (+/-) p=0,05</t>
   </si>
 </sst>
 </file>
@@ -910,7 +907,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -918,39 +915,39 @@
     <col min="1" max="1" width="24.42578125" customWidth="1"/>
     <col min="2" max="4" width="16.85546875" customWidth="1"/>
     <col min="5" max="5" width="26.5703125" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" customWidth="1"/>
+    <col min="6" max="6" width="36" customWidth="1"/>
     <col min="7" max="7" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C2" s="2">
         <v>400</v>
@@ -970,14 +967,26 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.73</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="G3" s="2">
+        <v>2622.81</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
kNN (250000 samples, k=12)
</commit_message>
<xml_diff>
--- a/report/Report.xlsx
+++ b/report/Report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
   <si>
     <t xml:space="preserve">Название метода </t>
   </si>
@@ -910,10 +910,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1063,6 +1063,29 @@
         <v>0.65</v>
       </c>
     </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2">
+        <v>250000</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.81</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>920.64</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
PCA + linear SVM
</commit_message>
<xml_diff>
--- a/report/Report.xlsx
+++ b/report/Report.xlsx
@@ -7,14 +7,15 @@
     <workbookView xWindow="240" yWindow="420" windowWidth="23715" windowHeight="9495"/>
   </bookViews>
   <sheets>
-    <sheet name="report" sheetId="1" r:id="rId1"/>
+    <sheet name="Тест по выборке из 5000" sheetId="1" r:id="rId1"/>
+    <sheet name="Остальные" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="14">
   <si>
     <t xml:space="preserve">Название метода </t>
   </si>
@@ -50,6 +51,12 @@
   </si>
   <si>
     <t>kNN (лидер)</t>
+  </si>
+  <si>
+    <t>RandomizedPCA+SVM</t>
+  </si>
+  <si>
+    <t>PCA(27, true), SVM(Linear, C=1)</t>
   </si>
 </sst>
 </file>
@@ -567,13 +574,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -910,22 +920,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.42578125" customWidth="1"/>
-    <col min="2" max="4" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" customWidth="1"/>
+    <col min="3" max="4" width="16.85546875" customWidth="1"/>
     <col min="5" max="5" width="26.5703125" customWidth="1"/>
-    <col min="6" max="6" width="36" customWidth="1"/>
+    <col min="6" max="6" width="29.28515625" customWidth="1"/>
     <col min="7" max="7" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" ht="28.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -941,7 +952,7 @@
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -1019,33 +1030,33 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2">
-        <v>250000</v>
+        <v>5000</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="2">
-        <v>0.8</v>
+        <v>0.78</v>
       </c>
       <c r="F5" s="2">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="G5" s="2">
-        <v>891.96</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="2">
         <v>12</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="C6" s="2">
         <v>5000</v>
@@ -1054,40 +1065,119 @@
         <v>8</v>
       </c>
       <c r="E6" s="2">
-        <v>0.78</v>
+        <v>0.74</v>
       </c>
       <c r="F6" s="2">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="G6" s="2">
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2">
-        <v>12</v>
-      </c>
-      <c r="C7" s="2">
-        <v>250000</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0.81</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0</v>
-      </c>
-      <c r="G7" s="2">
-        <v>920.64</v>
+        <v>6.87</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="27.5703125" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" customWidth="1"/>
+    <col min="6" max="6" width="29.85546875" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="75">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2">
+        <v>250000</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2">
+        <v>891.96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2">
+        <v>250000</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.81</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>920.64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Chose the best param for linear SVM
</commit_message>
<xml_diff>
--- a/report/Report.xlsx
+++ b/report/Report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="15">
   <si>
     <t xml:space="preserve">Название метода </t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>PCA(27, true), SVM(Linear, C=1)</t>
+  </si>
+  <si>
+    <t>SVM (SVC) (лидер)</t>
   </si>
 </sst>
 </file>
@@ -920,10 +923,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -961,33 +964,33 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2">
-        <v>400</v>
+        <v>5000</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>0.68</v>
+        <v>0.73</v>
       </c>
       <c r="F2" s="2">
-        <v>0.06</v>
+        <v>0.02</v>
       </c>
       <c r="G2" s="2">
-        <v>228.79</v>
+        <v>2622.81</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
+        <v>10</v>
+      </c>
+      <c r="B3" s="2">
+        <v>5</v>
       </c>
       <c r="C3" s="2">
         <v>5000</v>
@@ -996,21 +999,21 @@
         <v>8</v>
       </c>
       <c r="E3" s="2">
-        <v>0.73</v>
+        <v>0.76</v>
       </c>
       <c r="F3" s="2">
         <v>0.02</v>
       </c>
       <c r="G3" s="2">
-        <v>2622.81</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2">
         <v>5000</v>
@@ -1019,21 +1022,21 @@
         <v>8</v>
       </c>
       <c r="E4" s="2">
-        <v>0.76</v>
+        <v>0.78</v>
       </c>
       <c r="F4" s="2">
         <v>0.02</v>
       </c>
       <c r="G4" s="2">
-        <v>0.49</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="2">
         <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="C5" s="2">
         <v>5000</v>
@@ -1042,35 +1045,12 @@
         <v>8</v>
       </c>
       <c r="E5" s="2">
-        <v>0.78</v>
+        <v>0.74</v>
       </c>
       <c r="F5" s="2">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="G5" s="2">
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="2">
-        <v>5000</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0.74</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="G6" s="2">
         <v>6.87</v>
       </c>
     </row>
@@ -1085,7 +1065,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1099,7 +1079,7 @@
     <col min="7" max="7" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="75">
+    <row r="1" spans="1:7" ht="30">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1124,25 +1104,25 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="2">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="C2" s="2">
-        <v>250000</v>
+        <v>400</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>0.8</v>
+        <v>0.68</v>
       </c>
       <c r="F2" s="2">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="G2" s="2">
-        <v>891.96</v>
+        <v>228.79</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1150,7 +1130,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="2">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2">
         <v>250000</v>
@@ -1159,23 +1139,37 @@
         <v>8</v>
       </c>
       <c r="E3" s="2">
-        <v>0.81</v>
+        <v>0.8</v>
       </c>
       <c r="F3" s="2">
         <v>0</v>
       </c>
       <c r="G3" s="2">
-        <v>920.64</v>
+        <v>891.96</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2">
+        <v>250000</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.81</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>920.64</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Chose the best param for SVM with rbf kernel
</commit_message>
<xml_diff>
--- a/report/Report.xlsx
+++ b/report/Report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="16">
   <si>
     <t xml:space="preserve">Название метода </t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>SVM (SVC) (лидер)</t>
+  </si>
+  <si>
+    <t>Rbf, C=1, gamma=0.0001</t>
   </si>
 </sst>
 </file>
@@ -923,10 +926,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1052,6 +1055,29 @@
       </c>
       <c r="G5" s="2">
         <v>6.87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.78</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="G6" s="2">
+        <v>10.199999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PCA + rbf SVM
</commit_message>
<xml_diff>
--- a/report/Report.xlsx
+++ b/report/Report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="17">
   <si>
     <t xml:space="preserve">Название метода </t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>Rbf, C=1, gamma=0.0001</t>
+  </si>
+  <si>
+    <t>PCA(26, true), SVM(rbf, C=1, gamma=0,0001)</t>
   </si>
 </sst>
 </file>
@@ -926,16 +929,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.42578125" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
     <col min="3" max="4" width="16.85546875" customWidth="1"/>
     <col min="5" max="5" width="26.5703125" customWidth="1"/>
     <col min="6" max="6" width="29.28515625" customWidth="1"/>
@@ -990,10 +993,10 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="2">
-        <v>5</v>
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C3" s="2">
         <v>5000</v>
@@ -1002,21 +1005,21 @@
         <v>8</v>
       </c>
       <c r="E3" s="2">
-        <v>0.76</v>
+        <v>0.78</v>
       </c>
       <c r="F3" s="2">
         <v>0.02</v>
       </c>
       <c r="G3" s="2">
-        <v>0.49</v>
+        <v>10.199999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2">
         <v>5000</v>
@@ -1025,21 +1028,21 @@
         <v>8</v>
       </c>
       <c r="E4" s="2">
-        <v>0.78</v>
+        <v>0.76</v>
       </c>
       <c r="F4" s="2">
         <v>0.02</v>
       </c>
       <c r="G4" s="2">
-        <v>0.65</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2">
         <v>12</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="C5" s="2">
         <v>5000</v>
@@ -1048,21 +1051,21 @@
         <v>8</v>
       </c>
       <c r="E5" s="2">
-        <v>0.74</v>
+        <v>0.78</v>
       </c>
       <c r="F5" s="2">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="G5" s="2">
-        <v>6.87</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C6" s="2">
         <v>5000</v>
@@ -1071,13 +1074,36 @@
         <v>8</v>
       </c>
       <c r="E6" s="2">
-        <v>0.78</v>
+        <v>0.74</v>
       </c>
       <c r="F6" s="2">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="G6" s="2">
-        <v>10.199999999999999</v>
+        <v>6.87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="G7" s="2">
+        <v>4.8099999999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Linear SVM: learn by one feature. Try 1
</commit_message>
<xml_diff>
--- a/report/Report.xlsx
+++ b/report/Report.xlsx
@@ -8,14 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="Тест по выборке из 5000" sheetId="1" r:id="rId1"/>
-    <sheet name="Остальные" sheetId="2" r:id="rId2"/>
+    <sheet name="По всем" sheetId="3" r:id="rId2"/>
+    <sheet name="Остальные" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="52">
   <si>
     <t xml:space="preserve">Название метода </t>
   </si>
@@ -72,6 +73,105 @@
   </si>
   <si>
     <t>PCA(10, true), kNN(k=12)</t>
+  </si>
+  <si>
+    <t>*Лидер означает, что проводился поиск наилучших параметров по сетке значений</t>
+  </si>
+  <si>
+    <t>SVM (SVC) (по столбцу № 1)</t>
+  </si>
+  <si>
+    <t>SVM (SVC) (по столбцу № 0)</t>
+  </si>
+  <si>
+    <t>SVM (SVC) (по столбцу № 2)</t>
+  </si>
+  <si>
+    <t>SVM (SVC) (по столбцу № 3)</t>
+  </si>
+  <si>
+    <t>SVM (SVC) (по столбцу № 4)</t>
+  </si>
+  <si>
+    <t>SVM (SVC) (по столбцу № 5)</t>
+  </si>
+  <si>
+    <t>SVM (SVC) (по столбцу № 6)</t>
+  </si>
+  <si>
+    <t>SVM (SVC) (по столбцу № 7)</t>
+  </si>
+  <si>
+    <t>SVM (SVC) (по столбцу № 8)</t>
+  </si>
+  <si>
+    <t>SVM (SVC) (по столбцу № 9)</t>
+  </si>
+  <si>
+    <t>SVM (SVC) (по столбцу № 10)</t>
+  </si>
+  <si>
+    <t>SVM (SVC) (по столбцу № 11)</t>
+  </si>
+  <si>
+    <t>SVM (SVC) (по столбцу № 12)</t>
+  </si>
+  <si>
+    <t>SVM (SVC) (по столбцу № 13)</t>
+  </si>
+  <si>
+    <t>SVM (SVC) (по столбцу № 14)</t>
+  </si>
+  <si>
+    <t>SVM (SVC) (по столбцу № 15)</t>
+  </si>
+  <si>
+    <t>SVM (SVC) (по столбцу № 16)</t>
+  </si>
+  <si>
+    <t>SVM (SVC) (по столбцу № 17)</t>
+  </si>
+  <si>
+    <t>SVM (SVC) (по столбцу № 18)</t>
+  </si>
+  <si>
+    <t>SVM (SVC) (по столбцу № 19)</t>
+  </si>
+  <si>
+    <t>SVM (SVC) (по столбцу № 20)</t>
+  </si>
+  <si>
+    <t>SVM (SVC) (по столбцу № 21)</t>
+  </si>
+  <si>
+    <t>SVM (SVC) (по столбцу № 23)</t>
+  </si>
+  <si>
+    <t>SVM (SVC) (по столбцу № 22)</t>
+  </si>
+  <si>
+    <t>SVM (SVC) (по столбцу № 24)</t>
+  </si>
+  <si>
+    <t>SVM (SVC) (по столбцу № 25)</t>
+  </si>
+  <si>
+    <t>SVM (SVC) (по столбцу № 26)</t>
+  </si>
+  <si>
+    <t>SVM (SVC) (по столбцу № 27)</t>
+  </si>
+  <si>
+    <t>SVM (SVC) (по столбцу № 28)</t>
+  </si>
+  <si>
+    <t>SVM (SVC) (по столбцу № 29)</t>
+  </si>
+  <si>
+    <t>18814.88</t>
+  </si>
+  <si>
+    <t>долго</t>
   </si>
 </sst>
 </file>
@@ -935,15 +1035,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
     <col min="2" max="2" width="40.7109375" customWidth="1"/>
     <col min="3" max="4" width="16.85546875" customWidth="1"/>
     <col min="5" max="5" width="26.5703125" customWidth="1"/>
@@ -951,7 +1051,7 @@
     <col min="7" max="7" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28.5" customHeight="1">
+    <row r="1" spans="1:9" ht="28.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -973,8 +1073,11 @@
       <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -997,7 +1100,7 @@
         <v>2622.81</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -1020,7 +1123,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:9">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -1043,7 +1146,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:9">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -1066,7 +1169,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:9">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -1089,7 +1192,7 @@
         <v>6.87</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:9">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -1112,7 +1215,7 @@
         <v>4.8099999999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:9">
       <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
@@ -1134,6 +1237,630 @@
       <c r="G8" s="2">
         <v>0.63</v>
       </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1874.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="G10" s="2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="G12" s="2">
+        <v>3436.85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="G13" s="2">
+        <v>1.98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.38</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="G14" s="2">
+        <v>23805.64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="G15" s="2">
+        <v>99.05</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1.37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="G18" s="2">
+        <v>2076.38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="G19" s="2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="G20" s="2">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="G21" s="2">
+        <v>1.29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="G22" s="2">
+        <v>37.479999999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="G23" s="2">
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="G24" s="2">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="G25" s="2">
+        <v>1494.93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="G26" s="2">
+        <v>1.29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="G27" s="2">
+        <v>1.17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1143,10 +1870,103 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" customWidth="1"/>
+    <col min="6" max="6" width="34.140625" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="30">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2">
+        <v>250000</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2">
+        <v>891.96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2">
+        <v>250000</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.81</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>920.64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1206,52 +2026,6 @@
         <v>228.79</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="2">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2">
-        <v>250000</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2">
-        <v>891.96</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="2">
-        <v>12</v>
-      </c>
-      <c r="C4" s="2">
-        <v>250000</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0.81</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2">
-        <v>920.64</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>